<commit_message>
Ajustando codigo con documentación
</commit_message>
<xml_diff>
--- a/PruebasDocs.xlsx
+++ b/PruebasDocs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PIPEPC\Downloads\digital_money_house\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76516D96-DEDB-43A4-B93D-C86050E72078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F0E163-B5A7-4110-BD73-BD419C5DBA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A9499B0-2AA5-42B7-BD4A-A0F1F170D3EA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
   <si>
     <t>ID</t>
   </si>
@@ -188,9 +188,6 @@
     <t>Ingresar el token y seguidamente en Body poner los datos de tarjeta a asignar</t>
   </si>
   <si>
-    <t>Registro Tarjetas</t>
-  </si>
-  <si>
     <t>201 Created</t>
   </si>
   <si>
@@ -201,6 +198,81 @@
   </si>
   <si>
     <t>El numero de la tarjeta debe de ser de 16 dígitos</t>
+  </si>
+  <si>
+    <t>Eliminar Tarjeta(s)</t>
+  </si>
+  <si>
+    <t>Registro Tarjeta(s)</t>
+  </si>
+  <si>
+    <t>Card not found with ID: 2</t>
+  </si>
+  <si>
+    <t>Card deleted successfully</t>
+  </si>
+  <si>
+    <t>Ingresar el token y seguidamente en Body no poner ID correcto de tarjeta a eliminar</t>
+  </si>
+  <si>
+    <t>Ingresar el token y seguidamente en Body no poner ID equivocado de tarjeta a eliminar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresar el token y seguidamente poner ID de la cuenta incorrecta de la tarjeta </t>
+  </si>
+  <si>
+    <t>La tarjeta no pertenece a la cuenta con ID: x</t>
+  </si>
+  <si>
+    <t>Sprint 3</t>
+  </si>
+  <si>
+    <t>Ver Actividad</t>
+  </si>
+  <si>
+    <t>Ingreso dinero</t>
+  </si>
+  <si>
+    <t>Obtener Tarjeta(s) Users</t>
+  </si>
+  <si>
+    <t>Ingresar el token y seguidamente poner el ID correcto de la cuenta a obtener tarjetas</t>
+  </si>
+  <si>
+    <t>Ingresar el token y seguidamente el ID incorrecto de un User no existente</t>
+  </si>
+  <si>
+    <t>Cuenta no encontrada con ID: x</t>
+  </si>
+  <si>
+    <t>Obtener Detalles tarjeta específica</t>
+  </si>
+  <si>
+    <t>Dinero</t>
+  </si>
+  <si>
+    <t>Indicar un id no registrado de user</t>
+  </si>
+  <si>
+    <t>Escribir un monto menor a  1</t>
+  </si>
+  <si>
+    <t>El monto debe ser mayor a 0</t>
+  </si>
+  <si>
+    <t>Escribrir amount y description en Params</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actividad </t>
+  </si>
+  <si>
+    <t>403 Forbidden</t>
+  </si>
+  <si>
+    <t>Ingresar el token valido y ID correcto del user</t>
+  </si>
+  <si>
+    <t>Ingresar el token valido y ID incorrecto del user o no registrado</t>
   </si>
 </sst>
 </file>
@@ -244,7 +316,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -359,11 +431,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -383,41 +464,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -753,19 +843,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63E4DA82-05A7-4105-A3AF-13FB036E3D46}">
-  <dimension ref="C2:I27"/>
+  <dimension ref="C2:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="11.42578125" style="4"/>
     <col min="4" max="4" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="74.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="77.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="11.42578125" style="4"/>
   </cols>
@@ -794,13 +884,13 @@
       </c>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -817,9 +907,9 @@
       </c>
     </row>
     <row r="4" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C4" s="11"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="13"/>
       <c r="F4" s="2" t="s">
         <v>14</v>
       </c>
@@ -834,9 +924,9 @@
       </c>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="11"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="7"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="2" t="s">
         <v>17</v>
       </c>
@@ -851,9 +941,9 @@
       </c>
     </row>
     <row r="6" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C6" s="11"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="2" t="s">
         <v>22</v>
       </c>
@@ -868,14 +958,14 @@
       </c>
     </row>
     <row r="7" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C7" s="11"/>
+      <c r="C7" s="12"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C8" s="11"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="13" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="6" t="s">
@@ -892,9 +982,9 @@
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C9" s="11"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="4" t="s">
         <v>29</v>
       </c>
@@ -909,9 +999,9 @@
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C10" s="11"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="7"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="6" t="s">
         <v>14</v>
       </c>
@@ -926,9 +1016,9 @@
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C11" s="11"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="7"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="6" t="s">
         <v>22</v>
       </c>
@@ -943,14 +1033,14 @@
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C12" s="11"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="11"/>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="12"/>
+      <c r="D13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="10" t="s">
         <v>34</v>
       </c>
       <c r="F13" s="2" t="s">
@@ -967,9 +1057,9 @@
       </c>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
@@ -984,13 +1074,13 @@
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
@@ -1016,13 +1106,13 @@
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="10" t="s">
         <v>38</v>
       </c>
       <c r="F17" s="2" t="s">
@@ -1039,9 +1129,9 @@
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="7"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="11"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="12"/>
       <c r="F18" s="2" t="s">
         <v>14</v>
       </c>
@@ -1056,9 +1146,9 @@
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="7"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="10"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="11"/>
       <c r="F19" s="3" t="s">
         <v>22</v>
       </c>
@@ -1073,20 +1163,20 @@
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C20" s="7"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="8"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="18"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C21" s="7"/>
-      <c r="D21" s="7" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="13" t="s">
         <v>46</v>
       </c>
       <c r="F21" s="2" t="s">
@@ -1103,9 +1193,9 @@
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="2" t="s">
         <v>14</v>
       </c>
@@ -1120,9 +1210,9 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1137,24 +1227,20 @@
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C24" s="7"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C25" s="7"/>
+      <c r="C25" s="13"/>
       <c r="D25" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>51</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>49</v>
@@ -1167,24 +1253,26 @@
       </c>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="7"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="10"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="I26" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C27" s="15"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="2" t="s">
         <v>17</v>
       </c>
@@ -1192,25 +1280,403 @@
         <v>49</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C37" s="9"/>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="13"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="13"/>
+      <c r="D41" s="16"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="13"/>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="13"/>
+      <c r="D43" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="13"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="H44" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I44" s="20" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="13"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="13"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+      <c r="I46" s="20"/>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="13"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+      <c r="I47" s="20"/>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C48" s="13"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+      <c r="I48" s="20"/>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="13"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="13"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="13"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+      <c r="I51" s="20"/>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C52" s="13"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+      <c r="I52" s="20"/>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C53" s="13"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+      <c r="I53" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="21">
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E25:E28"/>
+    <mergeCell ref="D25:D36"/>
+    <mergeCell ref="C17:C36"/>
+    <mergeCell ref="C39:C53"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="E29:E32"/>
+    <mergeCell ref="E35:E36"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="C3:C14"/>
     <mergeCell ref="E21:E23"/>
     <mergeCell ref="D21:D23"/>
-    <mergeCell ref="C17:C26"/>
     <mergeCell ref="E17:E19"/>
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="D20:I20"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
     <mergeCell ref="E8:E11"/>
     <mergeCell ref="D8:D11"/>
     <mergeCell ref="D3:D6"/>

</xml_diff>